<commit_message>
exporting excel product, properties y options listo. Falta variants y stock
</commit_message>
<xml_diff>
--- a/spec/fixtures/exported.xlsx
+++ b/spec/fixtures/exported.xlsx
@@ -71,25 +71,25 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="4.189887640449439"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="8.589887640449438"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.589887640449438"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.68988764044944"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.48988764044944"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="10.78988764044944"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="6.389887640449439"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="6.389887640449439"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="5.289887640449439"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="7.489887640449439"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.489887640449439"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="7.489887640449439"/>
     <col min="8" max="8" bestFit="true" customWidth="true" width="8.589887640449438"/>
     <col min="9" max="9" bestFit="true" customWidth="true" width="10.78988764044944"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="6.389887640449439"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="11.88988764044944"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="6.389887640449439"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="12.989887640449439"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="21.789887640449443"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="29.489887640449442"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="7.489887640449439"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="26.18988764044944"/>
     <col min="14" max="14" bestFit="true" customWidth="true" width="8.589887640449438"/>
   </cols>
   <sheetData>
@@ -162,6 +162,74 @@
       <c r="N1" s="0" t="inlineStr">
         <is>
           <t>Categorías</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>queque</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>en molde de cupcake</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>1500.0</v>
+      </c>
+      <c r="E2" s="0" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="F2" s="0" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="G2" s="0" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="H2" s="0" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="I2" s="0" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="J2" s="0" t="inlineStr">
+        <is>
+          <t>queque-en-molde-de-cupcake</t>
+        </is>
+      </c>
+      <c r="K2" s="0" t="inlineStr">
+        <is>
+          <t>Este es el mejor queque de Chile</t>
+        </is>
+      </c>
+      <c r="L2" s="0" t="inlineStr">
+        <is>
+          <t>TODO</t>
+        </is>
+      </c>
+      <c r="M2" s="0" t="inlineStr">
+        <is>
+          <t>2017-12-06 17:26:02 UTC</t>
+        </is>
+      </c>
+      <c r="N2" s="0" t="inlineStr">
+        <is>
+          <t>TODO</t>
         </is>
       </c>
     </row>
@@ -179,14 +247,14 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="10.78988764044944"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="9.68988764044944"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.88988764044944"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="5.289887640449439"/>
   </cols>
   <sheetData>
@@ -204,6 +272,36 @@
       <c r="C1" s="0" t="inlineStr">
         <is>
           <t>Valor</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>Hecho en casa</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>For real no fake</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -221,7 +319,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
@@ -229,7 +327,7 @@
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="10.78988764044944"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="7.489887640449439"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="6.389887640449439"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="17.38988764044944"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -246,6 +344,36 @@
       <c r="C1" s="0" t="inlineStr">
         <is>
           <t>Valores</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>Sabor</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>Nueces, Vainilla</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>Tamaño</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>estoy a dieta, gigante</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
export almost ready. Missing some TODO
</commit_message>
<xml_diff>
--- a/spec/fixtures/exported.xlsx
+++ b/spec/fixtures/exported.xlsx
@@ -7,7 +7,8 @@
     <sheet name="Propiedades" sheetId="2" r:id="rId5"/>
     <sheet name="Opciones" sheetId="3" r:id="rId6"/>
     <sheet name="Variantes" sheetId="4" r:id="rId7"/>
-    <sheet name="Stock" sheetId="5" r:id="rId8"/>
+    <sheet name="Ubicaciones" sheetId="5" r:id="rId8"/>
+    <sheet name="Stock" sheetId="6" r:id="rId9"/>
   </sheets>
 </workbook>
 </file>
@@ -391,7 +392,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
@@ -399,11 +400,11 @@
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="4.189887640449439"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="10.78988764044944"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.589887640449438"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="6.389887640449439"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="6.389887640449439"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="6.389887640449439"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="5.289887640449439"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="17.38988764044944"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.88988764044944"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.589887640449438"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.489887640449439"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="6.389887640449439"/>
     <col min="8" max="8" bestFit="true" customWidth="true" width="8.589887640449438"/>
     <col min="9" max="9" bestFit="true" customWidth="true" width="10.78988764044944"/>
   </cols>
@@ -453,6 +454,37 @@
         <is>
           <t>Profundidad</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>Nueces, estoy a dieta</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>12345678</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>2000.0</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>200.0</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>10.0</v>
       </c>
     </row>
   </sheetData>
@@ -469,7 +501,181 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="4.189887640449439"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="8.589887640449438"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.08988764044944"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.68988764044944"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="7.489887640449439"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="14.08988764044944"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="11.88988764044944"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="11.88988764044944"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="6.389887640449439"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="16.28988764044944"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="5.289887640449439"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="10.78988764044944"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="9.68988764044944"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="19.58988764044944"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="0" t="inlineStr">
+        <is>
+          <t>Nombre</t>
+        </is>
+      </c>
+      <c r="C1" s="0" t="inlineStr">
+        <is>
+          <t>Nombre Interno</t>
+        </is>
+      </c>
+      <c r="D1" s="0" t="inlineStr">
+        <is>
+          <t>Calle</t>
+        </is>
+      </c>
+      <c r="E1" s="0" t="inlineStr">
+        <is>
+          <t>Ciudad</t>
+        </is>
+      </c>
+      <c r="F1" s="0" t="inlineStr">
+        <is>
+          <t>Calle de referencia</t>
+        </is>
+      </c>
+      <c r="G1" s="0" t="inlineStr">
+        <is>
+          <t>Código Postal</t>
+        </is>
+      </c>
+      <c r="H1" s="0" t="inlineStr">
+        <is>
+          <t>Teléfono</t>
+        </is>
+      </c>
+      <c r="I1" s="0" t="inlineStr">
+        <is>
+          <t>País</t>
+        </is>
+      </c>
+      <c r="J1" s="0" t="inlineStr">
+        <is>
+          <t>Región</t>
+        </is>
+      </c>
+      <c r="K1" s="0" t="inlineStr">
+        <is>
+          <t>Activa</t>
+        </is>
+      </c>
+      <c r="L1" s="0" t="inlineStr">
+        <is>
+          <t>Por defecto</t>
+        </is>
+      </c>
+      <c r="M1" s="0" t="inlineStr">
+        <is>
+          <t>Backorderable</t>
+        </is>
+      </c>
+      <c r="N1" s="0" t="inlineStr">
+        <is>
+          <t>Propagar por todas las variantes</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>Isla Diamante</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>Central</t>
+        </is>
+      </c>
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>Playa 123</t>
+        </is>
+      </c>
+      <c r="E2" s="0" t="inlineStr">
+        <is>
+          <t>Til Til</t>
+        </is>
+      </c>
+      <c r="F2" s="0" t="inlineStr">
+        <is>
+          <t>Juan algo 234</t>
+        </is>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>12345</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>76543469</v>
+      </c>
+      <c r="I2" s="0" t="inlineStr">
+        <is>
+          <t>Chile</t>
+        </is>
+      </c>
+      <c r="J2" s="0" t="inlineStr">
+        <is>
+          <t>Región Metropolitana</t>
+        </is>
+      </c>
+      <c r="K2" s="0" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="L2" s="0" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M2" s="0" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+      <c r="N2" s="0" t="inlineStr">
+        <is>
+          <t>Sí</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <sheetCalcPr fullCalcOnLoad="true"/>
+  <printOptions verticalCentered="false" horizontalCentered="false" headings="false" gridLines="false"/>
+  <pageMargins right="0.75" left="0.75" bottom="1.0" top="1.0" footer="0.5" header="0.5"/>
+  <pageSetup/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <sheetPr>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
@@ -478,7 +684,7 @@
     <col min="1" max="1" bestFit="true" customWidth="true" width="10.78988764044944"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="8.589887640449438"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="7.489887640449439"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.489887640449439"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.68988764044944"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="9.68988764044944"/>
   </cols>
   <sheetData>
@@ -500,12 +706,31 @@
       </c>
       <c r="D1" s="0" t="inlineStr">
         <is>
-          <t>Ubicación</t>
+          <t>ID Ubicación</t>
         </is>
       </c>
       <c r="E1" s="0" t="inlineStr">
         <is>
           <t>Backorderable</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="0" t="inlineStr">
+        <is>
+          <t>Sí</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Sku, weight, etc ready for product with and without variants. Missing categories
</commit_message>
<xml_diff>
--- a/spec/fixtures/exported.xlsx
+++ b/spec/fixtures/exported.xlsx
@@ -82,7 +82,7 @@
     <col min="2" max="2" bestFit="true" customWidth="true" width="9.68988764044944"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="18.48988764044944"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="10.78988764044944"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="7.489887640449439"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="9.68988764044944"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="7.489887640449439"/>
     <col min="7" max="7" bestFit="true" customWidth="true" width="7.489887640449439"/>
     <col min="8" max="8" bestFit="true" customWidth="true" width="8.589887640449438"/>
@@ -183,30 +183,20 @@
       <c r="D2" s="0" t="n">
         <v>1500.0</v>
       </c>
-      <c r="E2" s="0" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="F2" s="0" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="G2" s="0" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="H2" s="0" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
-      </c>
-      <c r="I2" s="0" t="inlineStr">
-        <is>
-          <t>TODO</t>
-        </is>
+      <c r="E2" s="0" t="n">
+        <v>234566</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>123.0</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>132.0</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>134.0</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>234.0</v>
       </c>
       <c r="J2" s="0" t="inlineStr">
         <is>
@@ -248,14 +238,14 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="10.78988764044944"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.88988764044944"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.68988764044944"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="5.289887640449439"/>
   </cols>
   <sheetData>
@@ -273,36 +263,6 @@
       <c r="C1" s="0" t="inlineStr">
         <is>
           <t>Valor</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="inlineStr">
-        <is>
-          <t>Hecho en casa</t>
-        </is>
-      </c>
-      <c r="C2" s="0" t="inlineStr">
-        <is>
-          <t>Sí</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" s="0" t="inlineStr">
-        <is>
-          <t>For real no fake</t>
-        </is>
-      </c>
-      <c r="C3" s="0" t="inlineStr">
-        <is>
-          <t>No</t>
         </is>
       </c>
     </row>
@@ -320,7 +280,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
@@ -328,7 +288,7 @@
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="10.78988764044944"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="7.489887640449439"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="17.38988764044944"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="6.389887640449439"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -345,36 +305,6 @@
       <c r="C1" s="0" t="inlineStr">
         <is>
           <t>Valores</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="inlineStr">
-        <is>
-          <t>Sabor</t>
-        </is>
-      </c>
-      <c r="C2" s="0" t="inlineStr">
-        <is>
-          <t>Nueces, Vainilla</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" s="0" t="inlineStr">
-        <is>
-          <t>Tamaño</t>
-        </is>
-      </c>
-      <c r="C3" s="0" t="inlineStr">
-        <is>
-          <t>estoy a dieta, gigante</t>
         </is>
       </c>
     </row>
@@ -392,7 +322,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
@@ -400,11 +330,11 @@
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="4.189887640449439"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="10.78988764044944"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="17.38988764044944"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="11.88988764044944"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.589887640449438"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.489887640449439"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="6.389887640449439"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.589887640449438"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="6.389887640449439"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="6.389887640449439"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="6.389887640449439"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="5.289887640449439"/>
     <col min="8" max="8" bestFit="true" customWidth="true" width="8.589887640449438"/>
     <col min="9" max="9" bestFit="true" customWidth="true" width="10.78988764044944"/>
   </cols>
@@ -454,37 +384,6 @@
         <is>
           <t>Profundidad</t>
         </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" s="0" t="inlineStr">
-        <is>
-          <t>Nueces, estoy a dieta</t>
-        </is>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>12345678</v>
-      </c>
-      <c r="E2" s="0" t="n">
-        <v>2000.0</v>
-      </c>
-      <c r="F2" s="0" t="n">
-        <v>200.0</v>
-      </c>
-      <c r="G2" s="0" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="H2" s="0" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="I2" s="0" t="n">
-        <v>10.0</v>
       </c>
     </row>
   </sheetData>
@@ -501,7 +400,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
@@ -510,13 +409,13 @@
     <col min="1" max="1" bestFit="true" customWidth="true" width="4.189887640449439"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="8.589887640449438"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="14.08988764044944"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.68988764044944"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="5.289887640449439"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="7.489887640449439"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="14.08988764044944"/>
     <col min="7" max="7" bestFit="true" customWidth="true" width="11.88988764044944"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="11.88988764044944"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="6.389887640449439"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="16.28988764044944"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="9.68988764044944"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="5.289887640449439"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="8.589887640449438"/>
     <col min="11" max="11" bestFit="true" customWidth="true" width="5.289887640449439"/>
     <col min="12" max="12" bestFit="true" customWidth="true" width="10.78988764044944"/>
     <col min="13" max="13" bestFit="true" customWidth="true" width="9.68988764044944"/>
@@ -595,72 +494,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="inlineStr">
-        <is>
-          <t>Isla Diamante</t>
-        </is>
-      </c>
-      <c r="C2" s="0" t="inlineStr">
-        <is>
-          <t>Central</t>
-        </is>
-      </c>
-      <c r="D2" s="0" t="inlineStr">
-        <is>
-          <t>Playa 123</t>
-        </is>
-      </c>
-      <c r="E2" s="0" t="inlineStr">
-        <is>
-          <t>Til Til</t>
-        </is>
-      </c>
-      <c r="F2" s="0" t="inlineStr">
-        <is>
-          <t>Juan algo 234</t>
-        </is>
-      </c>
-      <c r="G2" s="0" t="n">
-        <v>12345</v>
-      </c>
-      <c r="H2" s="0" t="n">
-        <v>76543469</v>
-      </c>
-      <c r="I2" s="0" t="inlineStr">
-        <is>
-          <t>Chile</t>
-        </is>
-      </c>
-      <c r="J2" s="0" t="inlineStr">
-        <is>
-          <t>Región Metropolitana</t>
-        </is>
-      </c>
-      <c r="K2" s="0" t="inlineStr">
-        <is>
-          <t>Sí</t>
-        </is>
-      </c>
-      <c r="L2" s="0" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="M2" s="0" t="inlineStr">
-        <is>
-          <t>Sí</t>
-        </is>
-      </c>
-      <c r="N2" s="0" t="inlineStr">
-        <is>
-          <t>Sí</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="true"/>
   <printOptions verticalCentered="false" horizontalCentered="false" headings="false" gridLines="false"/>
@@ -675,7 +508,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
@@ -715,25 +548,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" s="0" t="inlineStr">
-        <is>
-          <t>Sí</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="true"/>
   <printOptions verticalCentered="false" horizontalCentered="false" headings="false" gridLines="false"/>

</xml_diff>